<commit_message>
implemented a communication between effekseer and material editor
</commit_message>
<xml_diff>
--- a/Dev/release/resources/EffekseerMaterialLanguages.xlsx
+++ b/Dev/release/resources/EffekseerMaterialLanguages.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A8ADF4-C880-4C26-AD78-C0894CE1DF49}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="118">
   <si>
     <t>en</t>
     <phoneticPr fontId="1"/>
@@ -41,10 +40,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>SaveAs</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Value</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -98,14 +93,6 @@
   </si>
   <si>
     <t>ファイル</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>読込</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>保存</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -507,13 +494,52 @@
   </si>
   <si>
     <t>Constant Image</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SaveAs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SaveAs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>名前を付けて保存</t>
+    <rPh sb="0" eb="2">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>読み込む</t>
+    <rPh sb="0" eb="1">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>New</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>新規</t>
+    <rPh sb="0" eb="2">
+      <t>シンキ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -651,23 +677,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -703,23 +712,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -895,11 +887,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C154"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -928,520 +920,524 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>84</v>
-      </c>
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>45</v>
-      </c>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A51" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="C54" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="1"/>
@@ -1835,17 +1831,17 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A133" s="1"/>
-      <c r="B133" s="2"/>
+      <c r="B133" s="1"/>
       <c r="C133" s="1"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1"/>
-      <c r="B134" s="1"/>
+      <c r="B134" s="2"/>
       <c r="C134" s="1"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A135" s="1"/>
-      <c r="B135" s="2"/>
+      <c r="B135" s="1"/>
       <c r="C135" s="1"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
@@ -1855,18 +1851,18 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A137" s="1"/>
-      <c r="B137" s="1"/>
+      <c r="B137" s="2"/>
+      <c r="C137" s="1"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
     </row>
-    <row r="139" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
-      <c r="C139" s="1"/>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
+    </row>
+    <row r="140" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -1891,30 +1887,30 @@
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A146" s="1"/>
-      <c r="B146" s="1"/>
-      <c r="C146" s="1"/>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A145" s="1"/>
+      <c r="B145" s="1"/>
+      <c r="C145" s="1"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A149" s="1"/>
-      <c r="B149" s="1"/>
-      <c r="C149" s="1"/>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A148" s="1"/>
+      <c r="B148" s="1"/>
+      <c r="C148" s="1"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A152" s="1"/>
-      <c r="B152" s="1"/>
-      <c r="C152" s="1"/>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A153" s="1"/>
@@ -1923,7 +1919,12 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A154" s="1"/>
+      <c r="B154" s="1"/>
       <c r="C154" s="1"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A155" s="1"/>
+      <c r="C155" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
implemented save dialog in the material editor
</commit_message>
<xml_diff>
--- a/Dev/release/resources/EffekseerMaterialLanguages.xlsx
+++ b/Dev/release/resources/EffekseerMaterialLanguages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="119">
   <si>
     <t>en</t>
     <phoneticPr fontId="1"/>
@@ -533,6 +533,10 @@
     <rPh sb="0" eb="2">
       <t>シンキ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>New</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -890,8 +894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -924,7 +928,9 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
fixed many things about the material editor
</commit_message>
<xml_diff>
--- a/Dev/release/resources/EffekseerMaterialLanguages.xlsx
+++ b/Dev/release/resources/EffekseerMaterialLanguages.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D6CAB5-B239-40FE-AA7E-40BB193BDFF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="127">
   <si>
     <t>en</t>
     <phoneticPr fontId="1"/>
@@ -537,13 +538,57 @@
   </si>
   <si>
     <t>New</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Starting</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>開始</t>
+    <rPh sb="0" eb="2">
+      <t>カイシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Starting_New</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Starting_Open</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>マテリアルを開く</t>
+    <rPh sb="6" eb="7">
+      <t>ヒラ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>新規マテリアルを作成する</t>
+    <rPh sb="0" eb="2">
+      <t>シンキ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>サクセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Create new material</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open a material</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -681,6 +726,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -716,6 +778,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -891,11 +970,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1461,19 +1540,37 @@
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
+      <c r="A59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
+      <c r="A60" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A61" s="1"/>

</xml_diff>

<commit_message>
rename in material editor
</commit_message>
<xml_diff>
--- a/Dev/release/resources/EffekseerMaterialLanguages.xlsx
+++ b/Dev/release/resources/EffekseerMaterialLanguages.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D6CAB5-B239-40FE-AA7E-40BB193BDFF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="192">
   <si>
     <t>en</t>
     <phoneticPr fontId="1"/>
@@ -41,10 +40,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Value</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Value1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -101,10 +96,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>値</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>値1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -228,9 +219,6 @@
     <t>Divide</t>
   </si>
   <si>
-    <t>FMod</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -278,10 +266,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FMod_Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Output_Name</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -303,18 +287,6 @@
   </si>
   <si>
     <t>Constant2_Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Param_Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Param1_Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Param4_Name</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -368,10 +340,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Append_Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Append</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -396,54 +364,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>UV_Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>UV</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Panner_Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Panner</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>画像座標</t>
-    <rPh sb="0" eb="2">
-      <t>ガゾウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ザヒョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>移動座標</t>
-    <rPh sb="0" eb="2">
-      <t>イドウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ザヒョウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Coordinate_Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Coordinate</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>座標</t>
-    <rPh sb="0" eb="2">
-      <t>ザヒョウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -461,14 +386,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ParamTexture_Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ConstantTexture_Name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>パラメーター画像</t>
     <rPh sb="6" eb="8">
       <t>ガゾウ</t>
@@ -582,13 +499,395 @@
   </si>
   <si>
     <t>Open a material</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UV座標</t>
+    <rPh sb="2" eb="4">
+      <t>ザヒョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MovingUV</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>移動UV座標</t>
+    <rPh sb="0" eb="2">
+      <t>イドウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ザヒョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AppendVector_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Constant3_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Constant4_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Constant3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Constant4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>定数3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>定数4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Model_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Model</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>モデル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Parameter_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Parameter1_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Parameter4_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CustomData1_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CustomData2_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CustomData1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CustomData2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カスタムデータ1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>カスタムデータ2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VertexNormalWS_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>頂点法線</t>
+    <rPh sb="0" eb="2">
+      <t>チョウテン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ホウセン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>頂点接線</t>
+    <rPh sb="0" eb="2">
+      <t>チョウテン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画素法線</t>
+    <rPh sb="0" eb="2">
+      <t>ガソ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ホウセン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PixelNormal</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VertexNormal</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VertexTangent</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PixelNormalWS_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VertexTangentWS_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fmod_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mod</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画像</t>
+    <rPh sb="0" eb="2">
+      <t>ガゾウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TextureObjectParameter_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TextureObject_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Image</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Texture_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TextureCoordinate_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>検索</t>
+    <rPh sb="0" eb="2">
+      <t>ケンサク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>出力</t>
+    <rPh sb="0" eb="2">
+      <t>シュツリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Output</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>V.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>V.2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>V.3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>V.4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Out.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>値</t>
+    <rPh sb="0" eb="1">
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>V.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Comment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Priority</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Priority</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>優先度</t>
+    <rPh sb="0" eb="3">
+      <t>ユウセンド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ConstValue1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ConstValue2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sampler</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sampler</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サンプラ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UVIndex</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UV Index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UV番号</t>
+    <rPh sb="2" eb="4">
+      <t>バンゴウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ShadingModel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ShadingModel</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Lit</t>
+  </si>
+  <si>
+    <t>Unlit</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>ConstSpeed</t>
+  </si>
+  <si>
+    <t>速度</t>
+    <rPh sb="0" eb="2">
+      <t>ソクド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ライティング</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>非ライティング</t>
+    <rPh sb="0" eb="1">
+      <t>ヒ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>シェーディング
+モデル</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Lang</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Desc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>名称</t>
+    <rPh sb="0" eb="2">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>説明</t>
+    <rPh sb="0" eb="2">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>言語</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンゴ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Lang.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -726,23 +1025,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -778,23 +1060,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -970,11 +1235,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C155"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1003,18 +1268,18 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -1025,18 +1290,18 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -1047,247 +1312,259 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>185</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>191</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>186</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>8</v>
+        <v>186</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>187</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>187</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>159</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>11</v>
+        <v>161</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>155</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
-        <v>65</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>156</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>157</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
-        <v>67</v>
+        <v>167</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>154</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>155</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>79</v>
+        <v>162</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>85</v>
+        <v>164</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>165</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>92</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>90</v>
+        <v>169</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>170</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>89</v>
+        <v>172</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>87</v>
+        <v>173</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>82</v>
+        <v>175</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>83</v>
+        <v>176</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>84</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>100</v>
+        <v>178</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>101</v>
+        <v>178</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>102</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>94</v>
+        <v>179</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>95</v>
+        <v>179</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>98</v>
+        <v>181</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>96</v>
+        <v>180</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>97</v>
+        <v>180</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>99</v>
+        <v>181</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
@@ -1297,242 +1574,254 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>39</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>62</v>
+        <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>43</v>
-      </c>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>44</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" s="1" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>46</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>47</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>18</v>
+        <v>139</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>48</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A52" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" s="1" t="s">
-        <v>105</v>
+        <v>147</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="1"/>
@@ -1541,66 +1830,96 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>119</v>
+        <v>52</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>120</v>
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>121</v>
+        <v>67</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>125</v>
+        <v>53</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>124</v>
+        <v>32</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A60" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+      <c r="A62" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="A63" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="A64" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
+      <c r="A66" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="1"/>
@@ -1608,29 +1927,59 @@
       <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="A68" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="A69" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
+      <c r="A70" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="A71" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="A72" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="1"/>
@@ -1643,60 +1992,87 @@
       <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
+      <c r="A75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="A76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="A77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="A78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+      <c r="A79" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
+      <c r="A80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
+      <c r="A81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-    </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
@@ -1713,19 +2089,37 @@
       <c r="C88" s="1"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
+      <c r="A89" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
+      <c r="A90" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
+      <c r="A91" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A92" s="1"/>
@@ -1939,7 +2333,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A134" s="1"/>
-      <c r="B134" s="2"/>
+      <c r="B134" s="1"/>
       <c r="C134" s="1"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.15">
@@ -1949,23 +2343,25 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A136" s="1"/>
-      <c r="B136" s="2"/>
+      <c r="B136" s="1"/>
       <c r="C136" s="1"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A137" s="1"/>
-      <c r="B137" s="2"/>
+      <c r="B137" s="1"/>
       <c r="C137" s="1"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A138" s="1"/>
       <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A139" s="1"/>
       <c r="B139" s="1"/>
-    </row>
-    <row r="140" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C139" s="1"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A140" s="1"/>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -1995,6 +2391,11 @@
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
     </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A146" s="1"/>
+      <c r="B146" s="1"/>
+      <c r="C146" s="1"/>
+    </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A147" s="1"/>
       <c r="B147" s="1"/>
@@ -2005,6 +2406,11 @@
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
     </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A149" s="1"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
+    </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A150" s="1"/>
       <c r="B150" s="1"/>
@@ -2015,6 +2421,11 @@
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
     </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A152" s="1"/>
+      <c r="B152" s="1"/>
+      <c r="C152" s="1"/>
+    </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A153" s="1"/>
       <c r="B153" s="1"/>
@@ -2027,7 +2438,145 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A155" s="1"/>
+      <c r="B155" s="1"/>
       <c r="C155" s="1"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A156" s="1"/>
+      <c r="B156" s="1"/>
+      <c r="C156" s="1"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A157" s="1"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A158" s="1"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="1"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A159" s="1"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A160" s="1"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="1"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A161" s="1"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A162" s="1"/>
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A163" s="1"/>
+      <c r="B163" s="1"/>
+      <c r="C163" s="1"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A164" s="1"/>
+      <c r="B164" s="1"/>
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A165" s="1"/>
+      <c r="B165" s="2"/>
+      <c r="C165" s="1"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A166" s="1"/>
+      <c r="B166" s="1"/>
+      <c r="C166" s="1"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A167" s="1"/>
+      <c r="B167" s="2"/>
+      <c r="C167" s="1"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A168" s="1"/>
+      <c r="B168" s="2"/>
+      <c r="C168" s="1"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A169" s="1"/>
+      <c r="B169" s="1"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A170" s="1"/>
+      <c r="B170" s="1"/>
+    </row>
+    <row r="171" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A171" s="1"/>
+      <c r="B171" s="1"/>
+      <c r="C171" s="1"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A172" s="1"/>
+      <c r="B172" s="1"/>
+      <c r="C172" s="1"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A173" s="1"/>
+      <c r="B173" s="1"/>
+      <c r="C173" s="1"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A174" s="1"/>
+      <c r="B174" s="1"/>
+      <c r="C174" s="1"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A175" s="1"/>
+      <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A176" s="1"/>
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A178" s="1"/>
+      <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A179" s="1"/>
+      <c r="B179" s="1"/>
+      <c r="C179" s="1"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A181" s="1"/>
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+      <c r="C182" s="1"/>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A184" s="1"/>
+      <c r="B184" s="1"/>
+      <c r="C184" s="1"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A185" s="1"/>
+      <c r="B185" s="1"/>
+      <c r="C185" s="1"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A186" s="1"/>
+      <c r="C186" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
improved many things in Material Editor
</commit_message>
<xml_diff>
--- a/Dev/release/resources/EffekseerMaterialLanguages.xlsx
+++ b/Dev/release/resources/EffekseerMaterialLanguages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="225">
   <si>
     <t>en</t>
     <phoneticPr fontId="1"/>
@@ -37,22 +37,6 @@
   </si>
   <si>
     <t>Save</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Value1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Value2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Value3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Value4</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -707,10 +691,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Output</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>V.1</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -728,10 +708,6 @@
   </si>
   <si>
     <t>Out.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Value</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -750,14 +726,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Comment</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Priority</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Priority</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -769,27 +737,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ConstValue1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ConstValue2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Sampler</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Sampler</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>サンプラ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>UVIndex</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -801,10 +753,6 @@
     <rPh sb="2" eb="4">
       <t>バンゴウ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ShadingModel</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -970,6 +918,228 @@
   </si>
   <si>
     <t>English</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Value_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Value1_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Value2_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Value3_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Value4_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ConstValue1_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ConstValue2_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Output_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Comment_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Priority_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sampler_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>UVIndex_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ShadingModel_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Lit_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Unlit_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Speed_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ConstSpeed_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Priority_Desc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The lower the priority, the higher the screen is shown in other editors.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>低い優先度ほど、他のエディタの画面の上の位置に表示されます。</t>
+    <rPh sb="0" eb="1">
+      <t>ヒク</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>ユウセンド</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ホカ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>ウエ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>イチ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sampler_Desc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Specify how to treat an out of image.
+Repeat - repeat from opposite side
+Clamp - maintain the color of edge</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画像の外の扱い方を指定します。
+Repeat - 反対側の端から繰り返します。
+Clamp - 端の色を維持します。</t>
+    <rPh sb="0" eb="2">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ソト</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>アツカ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ハンタイ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>ガワ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>ハシ</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>ク</t>
+    </rPh>
+    <rPh sb="34" eb="35">
+      <t>カエ</t>
+    </rPh>
+    <rPh sb="48" eb="49">
+      <t>ハジ</t>
+    </rPh>
+    <rPh sb="50" eb="51">
+      <t>イロ</t>
+    </rPh>
+    <rPh sb="52" eb="54">
+      <t>イジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Warning_WrongInputType</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Warning_WrongProperty</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Different samplers are 
+assigned in a same image.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>同じ画像に異なるサンプラが
+設定されています。</t>
+    <rPh sb="0" eb="1">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ガゾウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>セッテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロパティが無効です。</t>
+    <rPh sb="6" eb="8">
+      <t>ムコウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A propery is invalid</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Warning_DifferentSampler</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>An input type is invalid</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>入力の型が無効です。</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウリョク</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>カタ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ムコウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1325,10 +1495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C192"/>
+  <dimension ref="A1:C195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1357,18 +1527,18 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
@@ -1379,18 +1549,18 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
@@ -1401,40 +1571,40 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>200</v>
+        <v>187</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>202</v>
+        <v>189</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
@@ -1444,57 +1614,57 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
@@ -1514,483 +1684,483 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>159</v>
+        <v>192</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>6</v>
+        <v>193</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>194</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>195</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>9</v>
+        <v>196</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>199</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>162</v>
+        <v>201</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>164</v>
+        <v>202</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
-        <v>169</v>
+        <v>210</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>171</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
-        <v>175</v>
+        <v>213</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>176</v>
+        <v>214</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>184</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>177</v>
+        <v>204</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>179</v>
+        <v>205</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>180</v>
+        <v>206</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>61</v>
+        <v>208</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>47</v>
+        <v>166</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>25</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>209</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>48</v>
+        <v>167</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>26</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
-        <v>141</v>
+        <v>59</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>142</v>
+        <v>45</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
-        <v>78</v>
+        <v>137</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>84</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52" s="1" t="s">
-        <v>120</v>
+        <v>71</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>121</v>
+        <v>72</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>122</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A53" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>136</v>
+        <v>82</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>135</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>92</v>
+        <v>134</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A61" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="A63" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>31</v>
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>67</v>
+        <v>141</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
@@ -2000,284 +2170,296 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A69" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>118</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>115</v>
+        <v>66</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>119</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="A73" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>58</v>
+        <v>112</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A76" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>128</v>
+        <v>54</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>130</v>
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>129</v>
+        <v>55</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>131</v>
+        <v>34</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+      <c r="A79" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
+      <c r="A80" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>11</v>
+        <v>125</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A82" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>41</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
+      <c r="A88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A95" s="1" t="s">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A98" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A99" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A100" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A96" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A97" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A101" s="1"/>
@@ -2285,19 +2467,37 @@
       <c r="C101" s="1"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
+      <c r="A102" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
+      <c r="A103" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A104" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A105" s="1"/>
@@ -2631,7 +2831,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A171" s="1"/>
-      <c r="B171" s="2"/>
+      <c r="B171" s="1"/>
       <c r="C171" s="1"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.15">
@@ -2641,7 +2841,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A173" s="1"/>
-      <c r="B173" s="2"/>
+      <c r="B173" s="1"/>
       <c r="C173" s="1"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.15">
@@ -2652,27 +2852,27 @@
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A175" s="1"/>
       <c r="B175" s="1"/>
+      <c r="C175" s="1"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A176" s="1"/>
-      <c r="B176" s="1"/>
-    </row>
-    <row r="177" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B176" s="2"/>
+      <c r="C176" s="1"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A177" s="1"/>
-      <c r="B177" s="1"/>
+      <c r="B177" s="2"/>
       <c r="C177" s="1"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
-      <c r="C178" s="1"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
-      <c r="C179" s="1"/>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.15">
+    </row>
+    <row r="180" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -2687,6 +2887,11 @@
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
     </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A183" s="1"/>
+      <c r="B183" s="1"/>
+      <c r="C183" s="1"/>
+    </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
@@ -2717,9 +2922,19 @@
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A192" s="1"/>
-      <c r="C192" s="1"/>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A193" s="1"/>
+      <c r="B193" s="1"/>
+      <c r="C193" s="1"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A194" s="1"/>
+      <c r="B194" s="1"/>
+      <c r="C194" s="1"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A195" s="1"/>
+      <c r="C195" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
added vertex color in the material
</commit_message>
<xml_diff>
--- a/Dev/release/resources/EffekseerMaterialLanguages.xlsx
+++ b/Dev/release/resources/EffekseerMaterialLanguages.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="258">
   <si>
     <t>en</t>
     <phoneticPr fontId="1"/>
@@ -494,16 +494,6 @@
   </si>
   <si>
     <t>MovingUV</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>移動UV座標</t>
-    <rPh sb="0" eb="2">
-      <t>イドウ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ザヒョウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1140,6 +1130,196 @@
     <rPh sb="5" eb="7">
       <t>ムコウ</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VertexColor</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VertexColor_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>頂点色</t>
+    <rPh sb="0" eb="2">
+      <t>チョウテン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>イロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>移動UV座標</t>
+    <rPh sb="4" eb="6">
+      <t>ザヒョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>切り上げ</t>
+    <rPh sb="0" eb="1">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ア</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Round up</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Round down</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>切り捨て</t>
+    <rPh sb="0" eb="1">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Decimal part</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>少数部</t>
+    <rPh sb="0" eb="2">
+      <t>ショウスウ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ceil_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Floor_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Frac_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Min_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Max_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Minimum</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Maximum</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>最小</t>
+    <rPh sb="0" eb="2">
+      <t>サイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>最大</t>
+    <rPh sb="0" eb="2">
+      <t>サイダイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Power_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SquareRoot_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>乗数</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Power</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SquareRoot</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>平方根</t>
+    <rPh sb="0" eb="3">
+      <t>ヘイホウコン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DotProduct_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CrossProduct_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dot</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cross</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>内積</t>
+    <rPh sb="0" eb="1">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>セキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>外積</t>
+    <rPh sb="0" eb="2">
+      <t>ガイセキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>線形補完</t>
+    <rPh sb="0" eb="2">
+      <t>センケイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ホカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LinearInterporate_Name</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LinearInterporate</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1495,10 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C205"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B79" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1576,35 +1756,35 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>189</v>
-      </c>
       <c r="C9" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
@@ -1614,57 +1794,57 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
@@ -1684,21 +1864,21 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>16</v>
@@ -1706,10 +1886,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>17</v>
@@ -1717,10 +1897,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -1728,10 +1908,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>19</v>
@@ -1739,10 +1919,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>16</v>
@@ -1750,10 +1930,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>17</v>
@@ -1761,7 +1941,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
@@ -1772,21 +1952,21 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
@@ -1794,57 +1974,57 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
@@ -1854,57 +2034,57 @@
     </row>
     <row r="35" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
@@ -1969,10 +2149,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>26</v>
@@ -2007,7 +2187,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>79</v>
@@ -2039,226 +2219,244 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="A53" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
-        <v>116</v>
+        <v>236</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>117</v>
+        <v>232</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>118</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>144</v>
+        <v>237</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>82</v>
+        <v>239</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>106</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A57" s="1" t="s">
-        <v>83</v>
+        <v>238</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>107</v>
+        <v>240</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>108</v>
+        <v>242</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A58" s="1" t="s">
-        <v>128</v>
+        <v>243</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>133</v>
+        <v>246</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>129</v>
+        <v>245</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A59" s="1" t="s">
-        <v>135</v>
+        <v>244</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>132</v>
+        <v>247</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>131</v>
+        <v>248</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A60" s="1" t="s">
-        <v>136</v>
+        <v>249</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>134</v>
+        <v>251</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>130</v>
+        <v>253</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A62" s="1" t="s">
-        <v>143</v>
+        <v>256</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>142</v>
+        <v>257</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>139</v>
+        <v>255</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A63" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A64" s="1" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>86</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A65" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
+      <c r="A66" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A67" s="1" t="s">
-        <v>62</v>
+        <v>127</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>48</v>
+        <v>132</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>27</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A68" s="1" t="s">
-        <v>63</v>
+        <v>134</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>49</v>
+        <v>131</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>28</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="A69" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A70" s="1" t="s">
-        <v>64</v>
+        <v>225</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>50</v>
+        <v>224</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>29</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A71" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>30</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A72" s="1" t="s">
-        <v>66</v>
+        <v>142</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>31</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A73" s="1" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A74" s="1" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>114</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A75" s="1" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>115</v>
+        <v>87</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.15">
@@ -2268,197 +2466,242 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A77" s="1" t="s">
-        <v>119</v>
+        <v>62</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A78" s="1" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A79" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A80" s="1" t="s">
-        <v>122</v>
+        <v>64</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>124</v>
+        <v>50</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>126</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
-        <v>123</v>
+        <v>65</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>125</v>
+        <v>51</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>127</v>
+        <v>30</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
+      <c r="A82" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
+      <c r="A83" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A84" s="1" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>7</v>
+        <v>111</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>36</v>
+        <v>113</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A85" s="1" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>8</v>
+        <v>112</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>37</v>
+        <v>114</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A86" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>38</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A87" s="1" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A88" s="1" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A89" s="1" t="s">
-        <v>12</v>
+        <v>120</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A90" s="1" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>13</v>
+        <v>123</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
+      <c r="A91" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
+      <c r="A95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
+      <c r="A96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
+      <c r="A97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A98" s="1" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>99</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A99" s="1" t="s">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>103</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A100" s="1" t="s">
-        <v>101</v>
+        <v>13</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.15">
@@ -2466,39 +2709,6 @@
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A102" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A103" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="27" x14ac:dyDescent="0.15">
-      <c r="A104" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A105" s="1"/>
       <c r="B105" s="1"/>
@@ -2515,19 +2725,37 @@
       <c r="C107" s="1"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
+      <c r="A108" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
+      <c r="A109" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
+      <c r="A110" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A111" s="1"/>
@@ -2535,19 +2763,37 @@
       <c r="C111" s="1"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
+      <c r="A112" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
+      <c r="A113" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="27" x14ac:dyDescent="0.15">
+      <c r="A114" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A115" s="1"/>
@@ -2846,7 +3092,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A174" s="1"/>
-      <c r="B174" s="2"/>
+      <c r="B174" s="1"/>
       <c r="C174" s="1"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.15">
@@ -2856,23 +3102,25 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A176" s="1"/>
-      <c r="B176" s="2"/>
+      <c r="B176" s="1"/>
       <c r="C176" s="1"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A177" s="1"/>
-      <c r="B177" s="2"/>
+      <c r="B177" s="1"/>
       <c r="C177" s="1"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A178" s="1"/>
       <c r="B178" s="1"/>
+      <c r="C178" s="1"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A179" s="1"/>
       <c r="B179" s="1"/>
-    </row>
-    <row r="180" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C179" s="1"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A180" s="1"/>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -2894,7 +3142,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A184" s="1"/>
-      <c r="B184" s="1"/>
+      <c r="B184" s="2"/>
       <c r="C184" s="1"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.15">
@@ -2902,17 +3150,25 @@
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
     </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A186" s="1"/>
+      <c r="B186" s="2"/>
+      <c r="C186" s="1"/>
+    </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A187" s="1"/>
-      <c r="B187" s="1"/>
+      <c r="B187" s="2"/>
       <c r="C187" s="1"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A188" s="1"/>
       <c r="B188" s="1"/>
-      <c r="C188" s="1"/>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.15">
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A189" s="1"/>
+      <c r="B189" s="1"/>
+    </row>
+    <row r="190" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A190" s="1"/>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -2922,6 +3178,11 @@
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
     </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A192" s="1"/>
+      <c r="B192" s="1"/>
+      <c r="C192" s="1"/>
+    </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A193" s="1"/>
       <c r="B193" s="1"/>
@@ -2934,7 +3195,42 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A195" s="1"/>
+      <c r="B195" s="1"/>
       <c r="C195" s="1"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A197" s="1"/>
+      <c r="B197" s="1"/>
+      <c r="C197" s="1"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A198" s="1"/>
+      <c r="B198" s="1"/>
+      <c r="C198" s="1"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A200" s="1"/>
+      <c r="B200" s="1"/>
+      <c r="C200" s="1"/>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A201" s="1"/>
+      <c r="B201" s="1"/>
+      <c r="C201" s="1"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A203" s="1"/>
+      <c r="B203" s="1"/>
+      <c r="C203" s="1"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A204" s="1"/>
+      <c r="B204" s="1"/>
+      <c r="C204" s="1"/>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A205" s="1"/>
+      <c r="C205" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>